<commit_message>
BSTATS-150: Form to create a scoresheet.
</commit_message>
<xml_diff>
--- a/teams_STL_1961-roster_appearances.xlsx
+++ b/teams_STL_1961-roster_appearances.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="116">
   <si>
     <t>Name</t>
   </si>
@@ -1177,11 +1177,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AB43"/>
+  <dimension ref="A2:AB42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:XFD43"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -4365,86 +4370,6 @@
       </c>
       <c r="AB42" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>0</v>
-      </c>
-      <c r="B43" t="s">
-        <v>1</v>
-      </c>
-      <c r="D43" t="s">
-        <v>2</v>
-      </c>
-      <c r="E43" t="s">
-        <v>3</v>
-      </c>
-      <c r="F43" t="s">
-        <v>4</v>
-      </c>
-      <c r="G43" t="s">
-        <v>5</v>
-      </c>
-      <c r="H43" t="s">
-        <v>6</v>
-      </c>
-      <c r="I43" t="s">
-        <v>7</v>
-      </c>
-      <c r="J43" t="s">
-        <v>8</v>
-      </c>
-      <c r="K43" t="s">
-        <v>9</v>
-      </c>
-      <c r="L43" t="s">
-        <v>10</v>
-      </c>
-      <c r="M43" t="s">
-        <v>11</v>
-      </c>
-      <c r="N43" t="s">
-        <v>12</v>
-      </c>
-      <c r="O43" t="s">
-        <v>13</v>
-      </c>
-      <c r="P43" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>15</v>
-      </c>
-      <c r="R43" t="s">
-        <v>16</v>
-      </c>
-      <c r="S43" t="s">
-        <v>17</v>
-      </c>
-      <c r="T43" t="s">
-        <v>18</v>
-      </c>
-      <c r="U43" t="s">
-        <v>19</v>
-      </c>
-      <c r="V43" t="s">
-        <v>20</v>
-      </c>
-      <c r="W43" t="s">
-        <v>21</v>
-      </c>
-      <c r="X43" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y43" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z43" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA43" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>